<commit_message>
Adición de interesados y cambios en memoria
</commit_message>
<xml_diff>
--- a/Repositorio/Proyecto/DocumentosPropios/MatrizDeInteresados.xlsx
+++ b/Repositorio/Proyecto/DocumentosPropios/MatrizDeInteresados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\USC\Cuarto\XesPro\Proxecto\2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergy6rey\Documents\GitHub\PracticaXesPro_GrupoL\Repositorio\Proyecto\DocumentosPropios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763A5773-9BA6-4D82-9D6B-41E8258CF605}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FEE143-FF3F-4918-B4D0-99AE05D2EAB4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="205">
   <si>
     <t>IDENTIFICACIÓN</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Email: ja.taboada.fernandez@geisoft.com</t>
   </si>
   <si>
-    <t>Interesado 9</t>
-  </si>
-  <si>
     <t>DevQRCodeScanner</t>
   </si>
   <si>
@@ -216,12 +213,6 @@
     <t>Externo</t>
   </si>
   <si>
-    <t>Interesado 10</t>
-  </si>
-  <si>
-    <t>Ministeria de sanidad, consumo y bienestar</t>
-  </si>
-  <si>
     <t>España</t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>Planificación y estimación de costes</t>
   </si>
   <si>
-    <t>Interesado 18</t>
-  </si>
-  <si>
     <t>Sociedad Gallega de Medioambiente</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>Email:  administracion@sogama.es</t>
   </si>
   <si>
-    <t>Aporte de información</t>
-  </si>
-  <si>
     <t>Reducción del impacto medioambiental del proyecto y mejor eficiencia en la eliminación de residuos</t>
   </si>
   <si>
@@ -432,9 +417,6 @@
     <t>Medios de comunicación</t>
   </si>
   <si>
-    <t>n / a</t>
-  </si>
-  <si>
     <t>Potenciar buena imagen del producto</t>
   </si>
   <si>
@@ -444,9 +426,6 @@
     <t>Competidores del cliente</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Diferenciar al cliente de ellos</t>
   </si>
   <si>
@@ -486,15 +465,6 @@
     <t>Desarrollo satisfactorio del proyecto. Obtención de información útil del cliente.</t>
   </si>
   <si>
-    <t>Marketing 1</t>
-  </si>
-  <si>
-    <t>CEO 1</t>
-  </si>
-  <si>
-    <t>Responsable 1</t>
-  </si>
-  <si>
     <t>Empleados local</t>
   </si>
   <si>
@@ -525,44 +495,171 @@
     <t>Uso del sistema una vez esté en marcha. Satisfacción con el servicio ofrecido.</t>
   </si>
   <si>
-    <t>Proveedor 1</t>
-  </si>
-  <si>
-    <t>Proveedor 2</t>
-  </si>
-  <si>
-    <t>ProveedorHosteleria 1</t>
-  </si>
-  <si>
-    <t>ProveedorHosteleria 2</t>
-  </si>
-  <si>
-    <t>ProveedorHosteleria 3</t>
-  </si>
-  <si>
-    <t>Consultores1</t>
-  </si>
-  <si>
-    <t>Consultores 2</t>
-  </si>
-  <si>
     <t>Competidores</t>
   </si>
   <si>
-    <t>A. Vecinales</t>
+    <t>Aportar información relacionada con la eliminación de residuos</t>
+  </si>
+  <si>
+    <t>CEO cliente</t>
+  </si>
+  <si>
+    <t>Contacto empresa cliente</t>
+  </si>
+  <si>
+    <t>Proveedor TPV y NFC</t>
+  </si>
+  <si>
+    <t>Proveedor dispositivos electrónicos</t>
+  </si>
+  <si>
+    <t>Proveedor hosteleria de carnes</t>
+  </si>
+  <si>
+    <t>Proveedor hosteleria de alcohol</t>
+  </si>
+  <si>
+    <t>Proveedor hosteleria de snacks</t>
+  </si>
+  <si>
+    <t>Administración pública</t>
+  </si>
+  <si>
+    <t>Ministerio de sanidad, consumo y medioambiente</t>
+  </si>
+  <si>
+    <t>Socio instalador de QR</t>
+  </si>
+  <si>
+    <t>Consultores de proyectos de locales</t>
+  </si>
+  <si>
+    <t>Asociaciones Vecinales</t>
+  </si>
+  <si>
+    <t>Técnicos de medioambiente</t>
+  </si>
+  <si>
+    <t>BAJO</t>
+  </si>
+  <si>
+    <t>Encargado de marketing GEISOFT</t>
+  </si>
+  <si>
+    <t>Compañía eléctrica</t>
+  </si>
+  <si>
+    <t>Asociaciones Tecnológicas</t>
+  </si>
+  <si>
+    <t>Instalador de Alarmas</t>
+  </si>
+  <si>
+    <t>Locales Nocturnos</t>
+  </si>
+  <si>
+    <t>Distribuidores locales</t>
+  </si>
+  <si>
+    <t>Análisis y diseño del sistema</t>
+  </si>
+  <si>
+    <t>Asociaciones sin ánimo de lucro</t>
+  </si>
+  <si>
+    <t>Proveedor de electricidad</t>
+  </si>
+  <si>
+    <t>Clientes no individuales</t>
+  </si>
+  <si>
+    <t>Especialista en seguridad perimetral</t>
+  </si>
+  <si>
+    <t>Transportistas de productos alimenticios perecederos</t>
+  </si>
+  <si>
+    <t>Competidores de otros sectores</t>
+  </si>
+  <si>
+    <t>Otros comercios cercanos</t>
+  </si>
+  <si>
+    <t>Santiago de Compostela (radio de 100 metros en torno a bar)</t>
+  </si>
+  <si>
+    <t>Comerciantes ubicados cerca del bar</t>
+  </si>
+  <si>
+    <t>Unión Fenosa</t>
+  </si>
+  <si>
+    <t>Securitas Direct</t>
+  </si>
+  <si>
+    <t>Email:  portavoz_comercial_empresarial@fenosa.es</t>
+  </si>
+  <si>
+    <t>Email:  auditoria_seguridad_empresas@securitas.com</t>
+  </si>
+  <si>
+    <t>N / A</t>
+  </si>
+  <si>
+    <t>Proporcionar energía eléctrica para los dispositivos eléctricos y electrónicos del nuevo sistema</t>
+  </si>
+  <si>
+    <t>Obtención de electricidad constante y de calidad para todos los dispotivos del local</t>
+  </si>
+  <si>
+    <t>Obtener clientes y celebrar congresos y otros actos festivos en el bar</t>
+  </si>
+  <si>
+    <t>Obtención de clientela adicional e interesada en la tecnología del local y publicidad de actos</t>
+  </si>
+  <si>
+    <t>Aumentar la seguridad del local</t>
+  </si>
+  <si>
+    <t>Creación de una seguridad de tipo físico y perimetral para el sistema y sus activos</t>
+  </si>
+  <si>
+    <t>Transportar las mercancías y productos perecederos necesarios para el funcionamiento del local</t>
+  </si>
+  <si>
+    <t>Recibimiento de productos en tiempo y forma adecuados a las necesidades del local</t>
+  </si>
+  <si>
+    <t>Adecuar sus horarios a los del bar</t>
+  </si>
+  <si>
+    <t>Compartición de cliente mediante la coordinación en cuanto a horarios y servicios</t>
+  </si>
+  <si>
+    <t>Convivir de forma adecuada con el bar</t>
+  </si>
+  <si>
+    <t>Obtener una relación agradable que permita a todos los comercios de la zona funcionar de una forma adecuada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -594,20 +691,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,19 +743,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFE699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -715,6 +801,12 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -755,24 +847,21 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -781,38 +870,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,27 +904,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
+    <cellStyle name="40% - Énfasis6" xfId="2" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1284,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,8 +1384,8 @@
     <col min="3" max="3" width="16.21875"/>
     <col min="4" max="4" width="15.88671875"/>
     <col min="5" max="5" width="31.88671875"/>
-    <col min="6" max="6" width="24.88671875"/>
-    <col min="7" max="7" width="21.109375"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" customWidth="1"/>
     <col min="8" max="8" width="18.77734375"/>
     <col min="9" max="9" width="20"/>
     <col min="10" max="10" width="14"/>
@@ -1306,23 +1395,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="8"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1360,7 +1449,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1381,7 +1470,7 @@
       <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -1395,7 +1484,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1416,7 +1505,7 @@
       <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1430,7 +1519,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1451,7 +1540,7 @@
       <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1465,7 +1554,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1486,7 +1575,7 @@
       <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1500,7 +1589,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1519,9 +1608,9 @@
         <v>52</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H7" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1535,7 +1624,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1554,9 +1643,9 @@
         <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H8" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1570,7 +1659,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1605,8 +1694,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>153</v>
+      <c r="A10" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -1626,7 +1715,7 @@
       <c r="G10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1640,26 +1729,26 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>154</v>
+      <c r="A11" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>145</v>
+        <v>137</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>21</v>
@@ -1668,33 +1757,33 @@
         <v>22</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>155</v>
+      <c r="A12" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>21</v>
@@ -1703,587 +1792,796 @@
         <v>22</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>156</v>
+      <c r="A13" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>57</v>
+        <v>148</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>76</v>
+        <v>150</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="F24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K24" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="N27" s="15"/>
+    </row>
+    <row r="28" spans="1:14" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="D29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H30" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="21" t="s">
+      <c r="I30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="D31" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K31" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="1" t="s">
+    <row r="32" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K23" s="14" t="s">
+      <c r="C32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K32" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="1" t="s">
+    <row r="33" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I24" s="1" t="s">
+    </row>
+    <row r="34" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="N27" s="18"/>
-    </row>
-    <row r="28" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="K34" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="27"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2292,22 +2590,7 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
-      <formula>"ALTO"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
@@ -2321,8 +2604,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+      <formula>"ALTO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+      <formula>"ALTO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -2336,11 +2649,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2351,7 +2664,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
+  <conditionalFormatting sqref="H25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -2378,8 +2691,16 @@
     <hyperlink ref="E27" r:id="rId9" display="http://www.riosarela.org/" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E15" r:id="rId11" xr:uid="{82932D09-2CD0-4E1C-BD85-D1EF0CF797FB}"/>
+    <hyperlink ref="E29" r:id="rId12" display="Email:  administracion@sogama.es" xr:uid="{325E3697-82EC-4422-836A-89D0E92DB85E}"/>
+    <hyperlink ref="E30" r:id="rId13" display="Email:  administracion@sogama.es" xr:uid="{81EC342B-72A6-4BEA-AFAA-671C0B27D770}"/>
+    <hyperlink ref="E31" r:id="rId14" display="Email:  administracion@sogama.es" xr:uid="{77469BCA-DBF8-4A39-BB0D-E41219F62918}"/>
+    <hyperlink ref="E32" r:id="rId15" display="Email:  administracion@sogama.es" xr:uid="{57E0EBDB-CD52-4C5F-AAE8-D10D0802F551}"/>
+    <hyperlink ref="E33" r:id="rId16" display="Email:  administracion@sogama.es" xr:uid="{5F750937-2B5A-4D78-A09E-B4AFC1D2A539}"/>
+    <hyperlink ref="E26" r:id="rId17" display="Email:  administracion@sogama.es" xr:uid="{174F105A-F895-428C-997E-FDDEE0195831}"/>
+    <hyperlink ref="E24" r:id="rId18" display="Email:  administracion@sogama.es" xr:uid="{368AA3E9-7D55-4B82-8DC2-D7C8A6206673}"/>
+    <hyperlink ref="E34" r:id="rId19" display="Email:  administracion@sogama.es" xr:uid="{6ACE38E6-B4C9-49AB-8214-5A1B5456F958}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>